<commit_message>
Revert "Merge branch 'master' of https://github.com/YapHeo/3DProject"
This reverts commit 62d532f224a55b548eef4d76f79b6e619a4a128a, reversing
changes made to dd05751b23cf7b6f1d1ac51d214aba04004a7e1c.
</commit_message>
<xml_diff>
--- a/00.Document/03.PD문서/PD예산사용현황_180509_지현우.xlsx
+++ b/00.Document/03.PD문서/PD예산사용현황_180509_지현우.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\6kigs_18\Desktop\3DProject\00.Document\03.PD문서\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39C95A11-C82A-4D4F-8E00-E824785CE712}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{477B203F-475C-42C9-9924-1ECA52F0522B}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="7995" windowHeight="9675" xr2:uid="{0EC58B1F-1628-4B4C-A412-28D13A49912A}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="26">
   <si>
     <t>예산안 리스트</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -71,27 +71,63 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>합계</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>단위=원</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>사용현황</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>비고</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>잔액</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>구입일</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Horror Props (pack)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>컨텐츠(오브젝트)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.99$(6,504\)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Female Zombie E</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>컨텐츠(이벤트)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>12$(14,898\)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Krasue</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>9.99$(12,495\)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>맵(튜토리얼)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5$(6,526\)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Derelict Building2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>총액</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(단위=원)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -320,34 +356,19 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="26" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="26" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -369,40 +390,70 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="26" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="26" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -510,6 +561,200 @@
         <a:xfrm>
           <a:off x="3638550" y="3171826"/>
           <a:ext cx="2695575" cy="1638300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>40914</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>209549</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="그림 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{76AA130A-72D6-46C6-8475-AF3672D37DA3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3609975" y="4860564"/>
+          <a:ext cx="2733675" cy="1635485"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>666750</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>200025</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="그림 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{177A9E2A-E3B4-4481-BBE3-9B5193FEF60B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3619500" y="6505575"/>
+          <a:ext cx="2705100" cy="1657350"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>200025</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="그림 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{68D59624-BF75-417B-A8FA-B6FCE29097DF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3629025" y="8201025"/>
+          <a:ext cx="2714625" cy="1638300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="그림 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FAEB8BCD-A36F-4F59-ABBD-3F3FEEAD9EA2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3600451" y="9858375"/>
+          <a:ext cx="2762249" cy="1457325"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -818,10 +1063,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13BBF53F-0CF2-4B59-8CD8-7B5CBD8A01DA}">
-  <dimension ref="B6:O23"/>
+  <dimension ref="B6:P54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N23" sqref="N23"/>
+      <selection activeCell="R17" sqref="R17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -834,287 +1079,725 @@
     <col min="15" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B6" s="2" t="s">
+    <row r="6" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B6" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-    </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B7" s="22"/>
-      <c r="C7" s="22"/>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="22"/>
-      <c r="G7" s="22"/>
-      <c r="H7" s="22"/>
-      <c r="I7" s="22"/>
-      <c r="J7" s="22"/>
-      <c r="K7" s="22"/>
-      <c r="N7" s="24" t="s">
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="22"/>
+      <c r="I6" s="22"/>
+      <c r="J6" s="22"/>
+      <c r="K6" s="22"/>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B7" s="23"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="23"/>
+      <c r="I7" s="23"/>
+      <c r="J7" s="23"/>
+      <c r="K7" s="23"/>
+      <c r="N7" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="O7" s="19"/>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B8" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="I8" s="21"/>
+      <c r="J8" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="K8" s="21"/>
+      <c r="N8" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="O8" s="14">
+        <v>6602</v>
+      </c>
+    </row>
+    <row r="9" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B9" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="4"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="I9" s="25"/>
+      <c r="J9" s="20">
+        <v>43229</v>
+      </c>
+      <c r="K9" s="21"/>
+      <c r="N9" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="O9" s="14">
+        <v>6571</v>
+      </c>
+    </row>
+    <row r="10" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B10" s="16"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="25"/>
+      <c r="J10" s="21"/>
+      <c r="K10" s="21"/>
+      <c r="N10" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="O7" s="23"/>
-    </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B8" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5" t="s">
+      <c r="O10" s="14">
+        <v>6504</v>
+      </c>
+    </row>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B11" s="16"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="25"/>
+      <c r="J11" s="21"/>
+      <c r="K11" s="21"/>
+      <c r="N11" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="K8" s="5"/>
-      <c r="N8" s="25" t="s">
-        <v>6</v>
-      </c>
-      <c r="O8" s="26">
-        <v>6602</v>
-      </c>
-    </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B9" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" s="9"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="I9" s="6"/>
-      <c r="J9" s="27">
-        <v>43229</v>
-      </c>
-      <c r="K9" s="5"/>
-      <c r="N9" s="25" t="s">
+      <c r="O11" s="14">
+        <v>14898</v>
+      </c>
+    </row>
+    <row r="12" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B12" s="16"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="24"/>
+      <c r="I12" s="25"/>
+      <c r="J12" s="21"/>
+      <c r="K12" s="21"/>
+      <c r="N12" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="O12" s="14">
+        <v>12495</v>
+      </c>
+    </row>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B13" s="16"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="24"/>
+      <c r="I13" s="25"/>
+      <c r="J13" s="21"/>
+      <c r="K13" s="21"/>
+      <c r="N13" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="O13" s="14">
+        <v>6526</v>
+      </c>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B14" s="16"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="24"/>
+      <c r="I14" s="25"/>
+      <c r="J14" s="21"/>
+      <c r="K14" s="21"/>
+      <c r="N14" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="O14" s="32">
+        <f>SUM(O8:O13)</f>
+        <v>53596</v>
+      </c>
+      <c r="P14" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B15" s="17"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="24"/>
+      <c r="I15" s="25"/>
+      <c r="J15" s="21"/>
+      <c r="K15" s="21"/>
+    </row>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B16" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="O9" s="26">
-        <v>6571</v>
-      </c>
-    </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B10" s="18"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="5"/>
-      <c r="N10" s="25" t="s">
-        <v>11</v>
-      </c>
-      <c r="O10" s="26">
-        <f>SUM(O8:O9)</f>
-        <v>13173</v>
-      </c>
-    </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B11" s="18"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="5"/>
-      <c r="K11" s="5"/>
-      <c r="N11" s="25" t="s">
+      <c r="C16" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="4"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="I16" s="21"/>
+      <c r="J16" s="20">
+        <v>43214</v>
+      </c>
+      <c r="K16" s="21"/>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B17" s="16"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="26"/>
+      <c r="I17" s="21"/>
+      <c r="J17" s="21"/>
+      <c r="K17" s="21"/>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B18" s="16"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="26"/>
+      <c r="I18" s="21"/>
+      <c r="J18" s="21"/>
+      <c r="K18" s="21"/>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B19" s="16"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="26"/>
+      <c r="I19" s="21"/>
+      <c r="J19" s="21"/>
+      <c r="K19" s="21"/>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B20" s="16"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="26"/>
+      <c r="I20" s="21"/>
+      <c r="J20" s="21"/>
+      <c r="K20" s="21"/>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B21" s="16"/>
+      <c r="C21" s="16"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="26"/>
+      <c r="I21" s="21"/>
+      <c r="J21" s="21"/>
+      <c r="K21" s="21"/>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B22" s="16"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="26"/>
+      <c r="I22" s="21"/>
+      <c r="J22" s="21"/>
+      <c r="K22" s="21"/>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B23" s="17"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="26"/>
+      <c r="I23" s="21"/>
+      <c r="J23" s="21"/>
+      <c r="K23" s="21"/>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B24" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D24" s="30"/>
+      <c r="E24" s="30"/>
+      <c r="F24" s="30"/>
+      <c r="G24" s="30"/>
+      <c r="H24" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="O11" s="26">
-        <v>46827</v>
-      </c>
-    </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B12" s="18"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="5"/>
-      <c r="N12" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="O12" s="17" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B13" s="18"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="5"/>
-      <c r="K13" s="5"/>
-    </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B14" s="18"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="5"/>
-    </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B15" s="19"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="6"/>
-      <c r="J15" s="5"/>
-      <c r="K15" s="5"/>
-    </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B16" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="C16" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="D16" s="9"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="I16" s="5"/>
-      <c r="J16" s="27">
-        <v>43214</v>
-      </c>
-      <c r="K16" s="5"/>
-    </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B17" s="18"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="16"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
-      <c r="K17" s="5"/>
-    </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B18" s="18"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="16"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="5"/>
-    </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B19" s="18"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="13"/>
-      <c r="H19" s="16"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="5"/>
-      <c r="K19" s="5"/>
-    </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B20" s="18"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="16"/>
-      <c r="I20" s="5"/>
-      <c r="J20" s="5"/>
-      <c r="K20" s="5"/>
-    </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B21" s="18"/>
-      <c r="C21" s="18"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="13"/>
-      <c r="H21" s="16"/>
-      <c r="I21" s="5"/>
-      <c r="J21" s="5"/>
-      <c r="K21" s="5"/>
-    </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B22" s="18"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="16"/>
-      <c r="I22" s="5"/>
-      <c r="J22" s="5"/>
-      <c r="K22" s="5"/>
-    </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B23" s="19"/>
-      <c r="C23" s="19"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="15"/>
-      <c r="H23" s="16"/>
-      <c r="I23" s="5"/>
-      <c r="J23" s="5"/>
-      <c r="K23" s="5"/>
+      <c r="I24" s="21"/>
+      <c r="J24" s="20">
+        <v>43234</v>
+      </c>
+      <c r="K24" s="21"/>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B25" s="21"/>
+      <c r="C25" s="29"/>
+      <c r="D25" s="30"/>
+      <c r="E25" s="30"/>
+      <c r="F25" s="30"/>
+      <c r="G25" s="30"/>
+      <c r="H25" s="26"/>
+      <c r="I25" s="21"/>
+      <c r="J25" s="21"/>
+      <c r="K25" s="21"/>
+    </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B26" s="21"/>
+      <c r="C26" s="29"/>
+      <c r="D26" s="30"/>
+      <c r="E26" s="30"/>
+      <c r="F26" s="30"/>
+      <c r="G26" s="30"/>
+      <c r="H26" s="26"/>
+      <c r="I26" s="21"/>
+      <c r="J26" s="21"/>
+      <c r="K26" s="21"/>
+    </row>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B27" s="21"/>
+      <c r="C27" s="29"/>
+      <c r="D27" s="30"/>
+      <c r="E27" s="30"/>
+      <c r="F27" s="30"/>
+      <c r="G27" s="30"/>
+      <c r="H27" s="26"/>
+      <c r="I27" s="21"/>
+      <c r="J27" s="21"/>
+      <c r="K27" s="21"/>
+    </row>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B28" s="21"/>
+      <c r="C28" s="29"/>
+      <c r="D28" s="30"/>
+      <c r="E28" s="30"/>
+      <c r="F28" s="30"/>
+      <c r="G28" s="30"/>
+      <c r="H28" s="26"/>
+      <c r="I28" s="21"/>
+      <c r="J28" s="21"/>
+      <c r="K28" s="21"/>
+    </row>
+    <row r="29" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B29" s="21"/>
+      <c r="C29" s="29"/>
+      <c r="D29" s="30"/>
+      <c r="E29" s="30"/>
+      <c r="F29" s="30"/>
+      <c r="G29" s="30"/>
+      <c r="H29" s="26"/>
+      <c r="I29" s="21"/>
+      <c r="J29" s="21"/>
+      <c r="K29" s="21"/>
+    </row>
+    <row r="30" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B30" s="21"/>
+      <c r="C30" s="29"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="26"/>
+      <c r="I30" s="21"/>
+      <c r="J30" s="21"/>
+      <c r="K30" s="21"/>
+    </row>
+    <row r="31" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B31" s="21"/>
+      <c r="C31" s="29"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="26"/>
+      <c r="I31" s="21"/>
+      <c r="J31" s="21"/>
+      <c r="K31" s="21"/>
+    </row>
+    <row r="32" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B32" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="C32" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="D32" s="28"/>
+      <c r="E32" s="28"/>
+      <c r="F32" s="28"/>
+      <c r="G32" s="28"/>
+      <c r="H32" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="I32" s="21"/>
+      <c r="J32" s="20">
+        <v>43234</v>
+      </c>
+      <c r="K32" s="21"/>
+    </row>
+    <row r="33" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B33" s="21"/>
+      <c r="C33" s="21"/>
+      <c r="D33" s="30"/>
+      <c r="E33" s="30"/>
+      <c r="F33" s="30"/>
+      <c r="G33" s="30"/>
+      <c r="H33" s="21"/>
+      <c r="I33" s="21"/>
+      <c r="J33" s="21"/>
+      <c r="K33" s="21"/>
+    </row>
+    <row r="34" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B34" s="21"/>
+      <c r="C34" s="21"/>
+      <c r="D34" s="30"/>
+      <c r="E34" s="30"/>
+      <c r="F34" s="30"/>
+      <c r="G34" s="30"/>
+      <c r="H34" s="21"/>
+      <c r="I34" s="21"/>
+      <c r="J34" s="21"/>
+      <c r="K34" s="21"/>
+    </row>
+    <row r="35" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B35" s="21"/>
+      <c r="C35" s="21"/>
+      <c r="D35" s="30"/>
+      <c r="E35" s="30"/>
+      <c r="F35" s="30"/>
+      <c r="G35" s="30"/>
+      <c r="H35" s="21"/>
+      <c r="I35" s="21"/>
+      <c r="J35" s="21"/>
+      <c r="K35" s="21"/>
+    </row>
+    <row r="36" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B36" s="21"/>
+      <c r="C36" s="21"/>
+      <c r="D36" s="30"/>
+      <c r="E36" s="30"/>
+      <c r="F36" s="30"/>
+      <c r="G36" s="30"/>
+      <c r="H36" s="21"/>
+      <c r="I36" s="21"/>
+      <c r="J36" s="21"/>
+      <c r="K36" s="21"/>
+    </row>
+    <row r="37" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B37" s="21"/>
+      <c r="C37" s="21"/>
+      <c r="D37" s="30"/>
+      <c r="E37" s="30"/>
+      <c r="F37" s="30"/>
+      <c r="G37" s="30"/>
+      <c r="H37" s="21"/>
+      <c r="I37" s="21"/>
+      <c r="J37" s="21"/>
+      <c r="K37" s="21"/>
+    </row>
+    <row r="38" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B38" s="21"/>
+      <c r="C38" s="21"/>
+      <c r="D38" s="30"/>
+      <c r="E38" s="30"/>
+      <c r="F38" s="30"/>
+      <c r="G38" s="30"/>
+      <c r="H38" s="21"/>
+      <c r="I38" s="21"/>
+      <c r="J38" s="21"/>
+      <c r="K38" s="21"/>
+    </row>
+    <row r="39" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B39" s="21"/>
+      <c r="C39" s="21"/>
+      <c r="D39" s="31"/>
+      <c r="E39" s="31"/>
+      <c r="F39" s="31"/>
+      <c r="G39" s="31"/>
+      <c r="H39" s="21"/>
+      <c r="I39" s="21"/>
+      <c r="J39" s="21"/>
+      <c r="K39" s="21"/>
+    </row>
+    <row r="40" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B40" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="C40" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="D40" s="21"/>
+      <c r="E40" s="21"/>
+      <c r="F40" s="21"/>
+      <c r="G40" s="21"/>
+      <c r="H40" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="I40" s="21"/>
+      <c r="J40" s="20">
+        <v>43234</v>
+      </c>
+      <c r="K40" s="21"/>
+    </row>
+    <row r="41" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B41" s="21"/>
+      <c r="C41" s="21"/>
+      <c r="D41" s="21"/>
+      <c r="E41" s="21"/>
+      <c r="F41" s="21"/>
+      <c r="G41" s="21"/>
+      <c r="H41" s="21"/>
+      <c r="I41" s="21"/>
+      <c r="J41" s="21"/>
+      <c r="K41" s="21"/>
+    </row>
+    <row r="42" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B42" s="21"/>
+      <c r="C42" s="21"/>
+      <c r="D42" s="21"/>
+      <c r="E42" s="21"/>
+      <c r="F42" s="21"/>
+      <c r="G42" s="21"/>
+      <c r="H42" s="21"/>
+      <c r="I42" s="21"/>
+      <c r="J42" s="21"/>
+      <c r="K42" s="21"/>
+    </row>
+    <row r="43" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B43" s="21"/>
+      <c r="C43" s="21"/>
+      <c r="D43" s="21"/>
+      <c r="E43" s="21"/>
+      <c r="F43" s="21"/>
+      <c r="G43" s="21"/>
+      <c r="H43" s="21"/>
+      <c r="I43" s="21"/>
+      <c r="J43" s="21"/>
+      <c r="K43" s="21"/>
+    </row>
+    <row r="44" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B44" s="21"/>
+      <c r="C44" s="21"/>
+      <c r="D44" s="21"/>
+      <c r="E44" s="21"/>
+      <c r="F44" s="21"/>
+      <c r="G44" s="21"/>
+      <c r="H44" s="21"/>
+      <c r="I44" s="21"/>
+      <c r="J44" s="21"/>
+      <c r="K44" s="21"/>
+    </row>
+    <row r="45" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B45" s="21"/>
+      <c r="C45" s="21"/>
+      <c r="D45" s="21"/>
+      <c r="E45" s="21"/>
+      <c r="F45" s="21"/>
+      <c r="G45" s="21"/>
+      <c r="H45" s="21"/>
+      <c r="I45" s="21"/>
+      <c r="J45" s="21"/>
+      <c r="K45" s="21"/>
+    </row>
+    <row r="46" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B46" s="21"/>
+      <c r="C46" s="21"/>
+      <c r="D46" s="21"/>
+      <c r="E46" s="21"/>
+      <c r="F46" s="21"/>
+      <c r="G46" s="21"/>
+      <c r="H46" s="21"/>
+      <c r="I46" s="21"/>
+      <c r="J46" s="21"/>
+      <c r="K46" s="21"/>
+    </row>
+    <row r="47" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B47" s="21"/>
+      <c r="C47" s="21"/>
+      <c r="D47" s="15"/>
+      <c r="E47" s="15"/>
+      <c r="F47" s="15"/>
+      <c r="G47" s="15"/>
+      <c r="H47" s="21"/>
+      <c r="I47" s="21"/>
+      <c r="J47" s="21"/>
+      <c r="K47" s="21"/>
+    </row>
+    <row r="48" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B48" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="C48" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="D48" s="4"/>
+      <c r="E48" s="5"/>
+      <c r="F48" s="5"/>
+      <c r="G48" s="6"/>
+      <c r="H48" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="I48" s="21"/>
+      <c r="J48" s="20">
+        <v>43231</v>
+      </c>
+      <c r="K48" s="21"/>
+    </row>
+    <row r="49" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B49" s="21"/>
+      <c r="C49" s="29"/>
+      <c r="D49" s="7"/>
+      <c r="E49" s="2"/>
+      <c r="F49" s="2"/>
+      <c r="G49" s="8"/>
+      <c r="H49" s="26"/>
+      <c r="I49" s="21"/>
+      <c r="J49" s="21"/>
+      <c r="K49" s="21"/>
+    </row>
+    <row r="50" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B50" s="21"/>
+      <c r="C50" s="29"/>
+      <c r="D50" s="7"/>
+      <c r="E50" s="2"/>
+      <c r="F50" s="2"/>
+      <c r="G50" s="8"/>
+      <c r="H50" s="26"/>
+      <c r="I50" s="21"/>
+      <c r="J50" s="21"/>
+      <c r="K50" s="21"/>
+    </row>
+    <row r="51" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B51" s="21"/>
+      <c r="C51" s="29"/>
+      <c r="D51" s="7"/>
+      <c r="E51" s="2"/>
+      <c r="F51" s="2"/>
+      <c r="G51" s="8"/>
+      <c r="H51" s="26"/>
+      <c r="I51" s="21"/>
+      <c r="J51" s="21"/>
+      <c r="K51" s="21"/>
+    </row>
+    <row r="52" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B52" s="21"/>
+      <c r="C52" s="29"/>
+      <c r="D52" s="7"/>
+      <c r="E52" s="2"/>
+      <c r="F52" s="2"/>
+      <c r="G52" s="8"/>
+      <c r="H52" s="26"/>
+      <c r="I52" s="21"/>
+      <c r="J52" s="21"/>
+      <c r="K52" s="21"/>
+    </row>
+    <row r="53" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B53" s="21"/>
+      <c r="C53" s="29"/>
+      <c r="D53" s="7"/>
+      <c r="E53" s="2"/>
+      <c r="F53" s="2"/>
+      <c r="G53" s="8"/>
+      <c r="H53" s="26"/>
+      <c r="I53" s="21"/>
+      <c r="J53" s="21"/>
+      <c r="K53" s="21"/>
+    </row>
+    <row r="54" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B54" s="21"/>
+      <c r="C54" s="29"/>
+      <c r="D54" s="9"/>
+      <c r="E54" s="3"/>
+      <c r="F54" s="3"/>
+      <c r="G54" s="10"/>
+      <c r="H54" s="26"/>
+      <c r="I54" s="21"/>
+      <c r="J54" s="21"/>
+      <c r="K54" s="21"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="32">
+    <mergeCell ref="H48:I54"/>
+    <mergeCell ref="J48:K54"/>
+    <mergeCell ref="C48:C54"/>
+    <mergeCell ref="B48:B54"/>
+    <mergeCell ref="B40:B47"/>
+    <mergeCell ref="C40:C47"/>
+    <mergeCell ref="D40:G47"/>
+    <mergeCell ref="H40:I47"/>
+    <mergeCell ref="J40:K47"/>
+    <mergeCell ref="B32:B39"/>
+    <mergeCell ref="H32:I39"/>
+    <mergeCell ref="J32:K39"/>
+    <mergeCell ref="C32:C39"/>
+    <mergeCell ref="D32:G39"/>
+    <mergeCell ref="D24:G29"/>
+    <mergeCell ref="C24:C31"/>
+    <mergeCell ref="B24:B31"/>
+    <mergeCell ref="H24:I31"/>
+    <mergeCell ref="J24:K31"/>
     <mergeCell ref="B9:B15"/>
     <mergeCell ref="B16:B23"/>
     <mergeCell ref="C9:C15"/>
@@ -1131,6 +1814,7 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>